<commit_message>
Creazioni classi per gestione dei tirocini
Creazioni classi per gestione dei tirocini da parte del amministratore
</commit_message>
<xml_diff>
--- a/DB/DBDictionary_1.0.2.xlsx
+++ b/DB/DBDictionary_1.0.2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="189">
   <si>
     <t>Description</t>
   </si>
@@ -583,6 +583,9 @@
   </si>
   <si>
     <t>0 reject, 1 accept, 2 pending, 3 notSend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiave esterna verso la tabella Student </t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1076,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1228,6 +1231,60 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1237,15 +1294,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1273,50 +1321,12 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="115">
@@ -1856,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J128"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1877,41 +1887,41 @@
   <sheetData>
     <row r="1" spans="2:10" ht="13" customHeight="1"/>
     <row r="3" spans="2:10">
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
     </row>
     <row r="5" spans="2:10" ht="21" customHeight="1">
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
     </row>
     <row r="6" spans="2:10" ht="16" thickBot="1"/>
     <row r="7" spans="2:10" ht="21" thickBot="1">
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="99"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="85"/>
     </row>
     <row r="8" spans="2:10" ht="16" thickBot="1">
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="94" t="s">
+      <c r="C8" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="96"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="82"/>
       <c r="J8" s="15" t="s">
         <v>21</v>
       </c>
@@ -1920,14 +1930,14 @@
       <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="91" t="s">
+      <c r="C9" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="93"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="79"/>
       <c r="J9" s="15" t="s">
         <v>6</v>
       </c>
@@ -2104,14 +2114,14 @@
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="85" t="s">
+      <c r="C17" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="89"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="73"/>
       <c r="J17" s="15" t="s">
         <v>152</v>
       </c>
@@ -2120,14 +2130,14 @@
       <c r="B18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="73" t="s">
+      <c r="C18" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="76"/>
     </row>
     <row r="19" spans="2:10" ht="16" thickBot="1">
       <c r="B19" s="10" t="s">
@@ -2228,7 +2238,7 @@
       <c r="B24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="85" t="s">
+      <c r="C24" s="71" t="s">
         <v>28</v>
       </c>
       <c r="D24" s="86"/>
@@ -2241,14 +2251,14 @@
       <c r="B25" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="C25" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="76"/>
     </row>
     <row r="26" spans="2:10" ht="16" thickBot="1">
       <c r="B26" s="10" t="s">
@@ -2541,27 +2551,27 @@
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="85" t="s">
+      <c r="C39" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="88"/>
-      <c r="E39" s="88"/>
-      <c r="F39" s="88"/>
-      <c r="G39" s="88"/>
-      <c r="H39" s="89"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
+      <c r="G39" s="72"/>
+      <c r="H39" s="73"/>
     </row>
     <row r="40" spans="1:9" ht="16" thickBot="1">
       <c r="B40" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="73" t="s">
+      <c r="C40" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="74"/>
-      <c r="E40" s="74"/>
-      <c r="F40" s="74"/>
-      <c r="G40" s="74"/>
-      <c r="H40" s="75"/>
+      <c r="D40" s="75"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="76"/>
     </row>
     <row r="41" spans="1:9" ht="16" thickBot="1">
       <c r="B41" s="10" t="s">
@@ -2783,27 +2793,27 @@
       <c r="B51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="85" t="s">
+      <c r="C51" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="D51" s="88"/>
-      <c r="E51" s="88"/>
-      <c r="F51" s="88"/>
-      <c r="G51" s="88"/>
-      <c r="H51" s="89"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="72"/>
+      <c r="F51" s="72"/>
+      <c r="G51" s="72"/>
+      <c r="H51" s="73"/>
     </row>
     <row r="52" spans="2:8" ht="16" thickBot="1">
       <c r="B52" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="73" t="s">
+      <c r="C52" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="74"/>
-      <c r="G52" s="74"/>
-      <c r="H52" s="75"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="75"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="76"/>
     </row>
     <row r="53" spans="2:8" ht="16" thickBot="1">
       <c r="B53" s="10" t="s">
@@ -2979,27 +2989,27 @@
       <c r="B61" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="85" t="s">
+      <c r="C61" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="D61" s="88"/>
-      <c r="E61" s="88"/>
-      <c r="F61" s="88"/>
-      <c r="G61" s="88"/>
-      <c r="H61" s="89"/>
+      <c r="D61" s="72"/>
+      <c r="E61" s="72"/>
+      <c r="F61" s="72"/>
+      <c r="G61" s="72"/>
+      <c r="H61" s="73"/>
     </row>
     <row r="62" spans="2:8" ht="16" thickBot="1">
       <c r="B62" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C62" s="73" t="s">
+      <c r="C62" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="D62" s="74"/>
-      <c r="E62" s="74"/>
-      <c r="F62" s="74"/>
-      <c r="G62" s="74"/>
-      <c r="H62" s="75"/>
+      <c r="D62" s="75"/>
+      <c r="E62" s="75"/>
+      <c r="F62" s="75"/>
+      <c r="G62" s="75"/>
+      <c r="H62" s="76"/>
     </row>
     <row r="63" spans="2:8" ht="16" thickBot="1">
       <c r="B63" s="10" t="s">
@@ -3083,27 +3093,27 @@
       <c r="B67" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C67" s="85" t="s">
+      <c r="C67" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="D67" s="88"/>
-      <c r="E67" s="88"/>
-      <c r="F67" s="88"/>
-      <c r="G67" s="88"/>
-      <c r="H67" s="89"/>
+      <c r="D67" s="72"/>
+      <c r="E67" s="72"/>
+      <c r="F67" s="72"/>
+      <c r="G67" s="72"/>
+      <c r="H67" s="73"/>
     </row>
     <row r="68" spans="2:8" ht="16" thickBot="1">
       <c r="B68" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C68" s="73" t="s">
+      <c r="C68" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="74"/>
-      <c r="G68" s="74"/>
-      <c r="H68" s="75"/>
+      <c r="D68" s="75"/>
+      <c r="E68" s="75"/>
+      <c r="F68" s="75"/>
+      <c r="G68" s="75"/>
+      <c r="H68" s="76"/>
     </row>
     <row r="69" spans="2:8" ht="16" thickBot="1">
       <c r="B69" s="10" t="s">
@@ -3394,27 +3404,27 @@
       <c r="B82" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C82" s="85" t="s">
+      <c r="C82" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="D82" s="88"/>
-      <c r="E82" s="88"/>
-      <c r="F82" s="88"/>
-      <c r="G82" s="88"/>
-      <c r="H82" s="89"/>
+      <c r="D82" s="72"/>
+      <c r="E82" s="72"/>
+      <c r="F82" s="72"/>
+      <c r="G82" s="72"/>
+      <c r="H82" s="73"/>
     </row>
     <row r="83" spans="2:8" ht="16" thickBot="1">
       <c r="B83" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C83" s="73" t="s">
+      <c r="C83" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="D83" s="74"/>
-      <c r="E83" s="74"/>
-      <c r="F83" s="74"/>
-      <c r="G83" s="74"/>
-      <c r="H83" s="75"/>
+      <c r="D83" s="75"/>
+      <c r="E83" s="75"/>
+      <c r="F83" s="75"/>
+      <c r="G83" s="75"/>
+      <c r="H83" s="76"/>
     </row>
     <row r="84" spans="2:8" ht="16" thickBot="1">
       <c r="B84" s="10" t="s">
@@ -3490,27 +3500,27 @@
       <c r="B88" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C88" s="85" t="s">
+      <c r="C88" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="D88" s="88"/>
-      <c r="E88" s="88"/>
-      <c r="F88" s="88"/>
-      <c r="G88" s="88"/>
-      <c r="H88" s="89"/>
+      <c r="D88" s="72"/>
+      <c r="E88" s="72"/>
+      <c r="F88" s="72"/>
+      <c r="G88" s="72"/>
+      <c r="H88" s="73"/>
     </row>
     <row r="89" spans="2:8" ht="16" thickBot="1">
       <c r="B89" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C89" s="73" t="s">
+      <c r="C89" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="D89" s="74"/>
-      <c r="E89" s="74"/>
-      <c r="F89" s="74"/>
-      <c r="G89" s="74"/>
-      <c r="H89" s="75"/>
+      <c r="D89" s="75"/>
+      <c r="E89" s="75"/>
+      <c r="F89" s="75"/>
+      <c r="G89" s="75"/>
+      <c r="H89" s="76"/>
     </row>
     <row r="90" spans="2:8" ht="16" thickBot="1">
       <c r="B90" s="10" t="s">
@@ -3724,27 +3734,27 @@
       <c r="B100" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C100" s="70" t="s">
+      <c r="C100" s="88" t="s">
         <v>153</v>
       </c>
-      <c r="D100" s="71"/>
-      <c r="E100" s="71"/>
-      <c r="F100" s="71"/>
-      <c r="G100" s="71"/>
-      <c r="H100" s="72"/>
+      <c r="D100" s="89"/>
+      <c r="E100" s="89"/>
+      <c r="F100" s="89"/>
+      <c r="G100" s="89"/>
+      <c r="H100" s="90"/>
     </row>
     <row r="101" spans="2:8" ht="16" thickBot="1">
       <c r="B101" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C101" s="73" t="s">
+      <c r="C101" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="D101" s="74"/>
-      <c r="E101" s="74"/>
-      <c r="F101" s="74"/>
-      <c r="G101" s="74"/>
-      <c r="H101" s="75"/>
+      <c r="D101" s="75"/>
+      <c r="E101" s="75"/>
+      <c r="F101" s="75"/>
+      <c r="G101" s="75"/>
+      <c r="H101" s="76"/>
     </row>
     <row r="102" spans="2:8" ht="16" thickBot="1">
       <c r="B102" s="10" t="s">
@@ -3774,7 +3784,7 @@
         <v>154</v>
       </c>
       <c r="C103" s="42" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D103" s="41" t="s">
         <v>155</v>
@@ -3783,129 +3793,129 @@
         <v>1</v>
       </c>
       <c r="F103" s="42">
-        <v>45</v>
+        <v>2147483647</v>
       </c>
       <c r="G103" s="43" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="H103" s="42" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="104" spans="2:8" ht="16" thickBot="1">
-      <c r="B104" s="57" t="s">
+    <row r="104" spans="2:8">
+      <c r="B104" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="C104" s="101" t="s">
+        <v>15</v>
+      </c>
+      <c r="D104" s="100" t="s">
+        <v>188</v>
+      </c>
+      <c r="E104" s="101">
+        <v>0</v>
+      </c>
+      <c r="F104" s="101">
+        <v>45</v>
+      </c>
+      <c r="G104" s="102" t="s">
+        <v>134</v>
+      </c>
+      <c r="H104" s="101" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" ht="16" thickBot="1">
+      <c r="B105" s="57" t="s">
         <v>156</v>
       </c>
-      <c r="C104" s="51" t="s">
+      <c r="C105" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="D104" s="57" t="s">
+      <c r="D105" s="57" t="s">
         <v>158</v>
       </c>
-      <c r="E104" s="51">
+      <c r="E105" s="51">
         <v>0</v>
       </c>
-      <c r="F104" s="51" t="s">
+      <c r="F105" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="G104" s="51" t="s">
+      <c r="G105" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="H104" s="51" t="s">
+      <c r="H105" s="51" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="106" spans="2:8" ht="16" thickBot="1"/>
-    <row r="107" spans="2:8" ht="16" thickBot="1">
-      <c r="B107" s="44" t="s">
+    <row r="107" spans="2:8" ht="16" thickBot="1"/>
+    <row r="108" spans="2:8" ht="16" thickBot="1">
+      <c r="B108" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C107" s="82" t="s">
+      <c r="C108" s="97" t="s">
         <v>159</v>
       </c>
-      <c r="D107" s="83"/>
-      <c r="E107" s="83"/>
-      <c r="F107" s="83"/>
-      <c r="G107" s="83"/>
-      <c r="H107" s="84"/>
-    </row>
-    <row r="108" spans="2:8" ht="16" thickBot="1">
-      <c r="B108" s="45" t="s">
+      <c r="D108" s="98"/>
+      <c r="E108" s="98"/>
+      <c r="F108" s="98"/>
+      <c r="G108" s="98"/>
+      <c r="H108" s="99"/>
+    </row>
+    <row r="109" spans="2:8" ht="16" thickBot="1">
+      <c r="B109" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="79" t="s">
+      <c r="C109" s="94" t="s">
         <v>137</v>
       </c>
-      <c r="D108" s="80"/>
-      <c r="E108" s="80"/>
-      <c r="F108" s="80"/>
-      <c r="G108" s="80"/>
-      <c r="H108" s="81"/>
-    </row>
-    <row r="109" spans="2:8" ht="16" thickBot="1">
-      <c r="B109" s="46" t="s">
+      <c r="D109" s="95"/>
+      <c r="E109" s="95"/>
+      <c r="F109" s="95"/>
+      <c r="G109" s="95"/>
+      <c r="H109" s="96"/>
+    </row>
+    <row r="110" spans="2:8" ht="16" thickBot="1">
+      <c r="B110" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="D109" s="47" t="s">
+      <c r="C110" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D110" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E109" s="47" t="s">
+      <c r="E110" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F109" s="47" t="s">
+      <c r="F110" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G109" s="47" t="s">
+      <c r="G110" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="H109" s="47" t="s">
+      <c r="H110" s="47" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="110" spans="2:8">
-      <c r="B110" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="C110" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="D110" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="E110" s="49">
-        <v>1</v>
-      </c>
-      <c r="F110" s="49">
-        <v>2147483647</v>
-      </c>
-      <c r="G110" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="H110" s="49" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="111" spans="2:8">
       <c r="B111" s="48" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C111" s="49" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D111" s="50" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E111" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F111" s="49">
-        <v>45</v>
+        <v>2147483647</v>
       </c>
       <c r="G111" s="49" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="H111" s="49" t="s">
         <v>52</v>
@@ -3913,13 +3923,13 @@
     </row>
     <row r="112" spans="2:8">
       <c r="B112" s="48" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C112" s="49" t="s">
         <v>15</v>
       </c>
       <c r="D112" s="50" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E112" s="49">
         <v>0</v>
@@ -3934,253 +3944,253 @@
         <v>52</v>
       </c>
     </row>
-    <row r="113" spans="2:8" ht="16" thickBot="1">
-      <c r="B113" s="54" t="s">
+    <row r="113" spans="2:8">
+      <c r="B113" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C113" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D113" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="E113" s="49">
+        <v>0</v>
+      </c>
+      <c r="F113" s="49">
+        <v>45</v>
+      </c>
+      <c r="G113" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="H113" s="49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="114" spans="2:8" ht="16" thickBot="1">
+      <c r="B114" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="C113" s="55" t="s">
+      <c r="C114" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D113" s="56" t="s">
+      <c r="D114" s="56" t="s">
         <v>167</v>
       </c>
-      <c r="E113" s="55">
-        <v>1</v>
-      </c>
-      <c r="F113" s="51">
+      <c r="E114" s="55">
+        <v>1</v>
+      </c>
+      <c r="F114" s="51">
         <v>2147483647</v>
       </c>
-      <c r="G113" s="55" t="s">
+      <c r="G114" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="H113" s="55" t="s">
+      <c r="H114" s="55" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="114" spans="2:8" ht="16" thickBot="1"/>
-    <row r="115" spans="2:8" ht="16" thickBot="1">
-      <c r="B115" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C115" s="70" t="s">
-        <v>172</v>
-      </c>
-      <c r="D115" s="71"/>
-      <c r="E115" s="71"/>
-      <c r="F115" s="71"/>
-      <c r="G115" s="71"/>
-      <c r="H115" s="72"/>
-    </row>
+    <row r="115" spans="2:8" ht="16" thickBot="1"/>
     <row r="116" spans="2:8" ht="16" thickBot="1">
       <c r="B116" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C116" s="88" t="s">
+        <v>172</v>
+      </c>
+      <c r="D116" s="89"/>
+      <c r="E116" s="89"/>
+      <c r="F116" s="89"/>
+      <c r="G116" s="89"/>
+      <c r="H116" s="90"/>
+    </row>
+    <row r="117" spans="2:8" ht="16" thickBot="1">
+      <c r="B117" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C116" s="73" t="s">
+      <c r="C117" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="D116" s="74"/>
-      <c r="E116" s="74"/>
-      <c r="F116" s="74"/>
-      <c r="G116" s="74"/>
-      <c r="H116" s="75"/>
-    </row>
-    <row r="117" spans="2:8" ht="16" thickBot="1">
-      <c r="B117" s="10" t="s">
+      <c r="D117" s="75"/>
+      <c r="E117" s="75"/>
+      <c r="F117" s="75"/>
+      <c r="G117" s="75"/>
+      <c r="H117" s="76"/>
+    </row>
+    <row r="118" spans="2:8" ht="16" thickBot="1">
+      <c r="B118" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D117" s="4" t="s">
+      <c r="C118" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D118" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E117" s="4" t="s">
+      <c r="E118" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F117" s="4" t="s">
+      <c r="F118" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G117" s="4" t="s">
+      <c r="G118" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H117" s="4" t="s">
+      <c r="H118" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="118" spans="2:8">
-      <c r="B118" s="41" t="s">
+    <row r="119" spans="2:8">
+      <c r="B119" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="C118" s="42" t="s">
+      <c r="C119" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D118" s="41" t="s">
+      <c r="D119" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="E118" s="42">
-        <v>1</v>
-      </c>
-      <c r="F118" s="42">
+      <c r="E119" s="42">
+        <v>1</v>
+      </c>
+      <c r="F119" s="42">
         <v>2147483647</v>
       </c>
-      <c r="G118" s="42" t="s">
+      <c r="G119" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="H118" s="58" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="119" spans="2:8" ht="16" thickBot="1">
-      <c r="B119" s="57" t="s">
+      <c r="H119" s="58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="2:8" ht="16" thickBot="1">
+      <c r="B120" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="C119" s="51" t="s">
+      <c r="C120" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D119" s="57" t="s">
+      <c r="D120" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="E119" s="51">
+      <c r="E120" s="51">
         <v>0</v>
       </c>
-      <c r="F119" s="51">
+      <c r="F120" s="51">
         <v>45</v>
       </c>
-      <c r="G119" s="51" t="s">
+      <c r="G120" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="H119" s="59" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="120" spans="2:8" ht="16" thickBot="1"/>
-    <row r="121" spans="2:8" ht="16" thickBot="1">
-      <c r="B121" s="60" t="s">
+      <c r="H120" s="59" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="121" spans="2:8" ht="16" thickBot="1"/>
+    <row r="122" spans="2:8" ht="16" thickBot="1">
+      <c r="B122" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C121" s="76" t="s">
+      <c r="C122" s="91" t="s">
         <v>176</v>
       </c>
-      <c r="D121" s="77"/>
-      <c r="E121" s="77"/>
-      <c r="F121" s="77"/>
-      <c r="G121" s="77"/>
-      <c r="H121" s="78"/>
-    </row>
-    <row r="122" spans="2:8" ht="16" thickBot="1">
-      <c r="B122" s="45" t="s">
+      <c r="D122" s="92"/>
+      <c r="E122" s="92"/>
+      <c r="F122" s="92"/>
+      <c r="G122" s="92"/>
+      <c r="H122" s="93"/>
+    </row>
+    <row r="123" spans="2:8" ht="16" thickBot="1">
+      <c r="B123" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C122" s="79" t="s">
+      <c r="C123" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="D122" s="80"/>
-      <c r="E122" s="80"/>
-      <c r="F122" s="80"/>
-      <c r="G122" s="80"/>
-      <c r="H122" s="81"/>
-    </row>
-    <row r="123" spans="2:8" ht="16" thickBot="1">
-      <c r="B123" s="46" t="s">
+      <c r="D123" s="95"/>
+      <c r="E123" s="95"/>
+      <c r="F123" s="95"/>
+      <c r="G123" s="95"/>
+      <c r="H123" s="96"/>
+    </row>
+    <row r="124" spans="2:8" ht="16" thickBot="1">
+      <c r="B124" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C123" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="D123" s="47" t="s">
+      <c r="C124" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D124" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E123" s="47" t="s">
+      <c r="E124" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F123" s="47" t="s">
+      <c r="F124" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G123" s="47" t="s">
+      <c r="G124" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="H123" s="47" t="s">
+      <c r="H124" s="47" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="124" spans="2:8">
-      <c r="B124" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="C124" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="D124" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="E124" s="49">
-        <v>1</v>
-      </c>
-      <c r="F124" s="49">
-        <v>2147483647</v>
-      </c>
-      <c r="G124" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="H124" s="61" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="125" spans="2:8">
       <c r="B125" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="C125" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D125" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="E125" s="49">
+        <v>1</v>
+      </c>
+      <c r="F125" s="49">
+        <v>2147483647</v>
+      </c>
+      <c r="G125" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="H125" s="61" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="2:8">
+      <c r="B126" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C125" s="49" t="s">
+      <c r="C126" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="D125" s="50" t="s">
+      <c r="D126" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="E125" s="49">
+      <c r="E126" s="49">
         <v>0</v>
       </c>
-      <c r="F125" s="49">
+      <c r="F126" s="49">
         <v>45</v>
       </c>
-      <c r="G125" s="49" t="s">
+      <c r="G126" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="H125" s="61" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="126" spans="2:8">
-      <c r="B126" s="62" t="s">
-        <v>180</v>
-      </c>
-      <c r="C126" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="D126" s="64" t="s">
-        <v>181</v>
-      </c>
-      <c r="E126" s="63">
-        <v>1</v>
-      </c>
-      <c r="F126" s="49">
-        <v>2147483647</v>
-      </c>
-      <c r="G126" s="63" t="s">
-        <v>89</v>
-      </c>
-      <c r="H126" s="65" t="s">
+      <c r="H126" s="61" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="127" spans="2:8">
       <c r="B127" s="62" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C127" s="63" t="s">
         <v>16</v>
       </c>
       <c r="D127" s="64" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E127" s="63">
         <v>1</v>
@@ -4195,31 +4205,66 @@
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="2:8" ht="16" thickBot="1">
-      <c r="B128" s="66" t="s">
+    <row r="128" spans="2:8">
+      <c r="B128" s="62" t="s">
+        <v>182</v>
+      </c>
+      <c r="C128" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="D128" s="64" t="s">
+        <v>183</v>
+      </c>
+      <c r="E128" s="63">
+        <v>1</v>
+      </c>
+      <c r="F128" s="49">
+        <v>2147483647</v>
+      </c>
+      <c r="G128" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="H128" s="65" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" ht="16" thickBot="1">
+      <c r="B129" s="66" t="s">
         <v>184</v>
       </c>
-      <c r="C128" s="67" t="s">
+      <c r="C129" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D128" s="68" t="s">
+      <c r="D129" s="68" t="s">
         <v>185</v>
       </c>
-      <c r="E128" s="67">
-        <v>1</v>
-      </c>
-      <c r="F128" s="67">
+      <c r="E129" s="67">
+        <v>1</v>
+      </c>
+      <c r="F129" s="67">
         <v>2147483647</v>
       </c>
-      <c r="G128" s="67" t="s">
+      <c r="G129" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="H128" s="69" t="s">
+      <c r="H129" s="69" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C116:H116"/>
+    <mergeCell ref="C117:H117"/>
+    <mergeCell ref="C122:H122"/>
+    <mergeCell ref="C123:H123"/>
+    <mergeCell ref="C101:H101"/>
+    <mergeCell ref="C108:H108"/>
+    <mergeCell ref="C109:H109"/>
+    <mergeCell ref="C88:H88"/>
+    <mergeCell ref="C100:H100"/>
+    <mergeCell ref="C89:H89"/>
+    <mergeCell ref="C82:H82"/>
+    <mergeCell ref="C83:H83"/>
     <mergeCell ref="B3:C5"/>
     <mergeCell ref="C67:H67"/>
     <mergeCell ref="C68:H68"/>
@@ -4236,18 +4281,6 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C39:H39"/>
-    <mergeCell ref="C88:H88"/>
-    <mergeCell ref="C100:H100"/>
-    <mergeCell ref="C89:H89"/>
-    <mergeCell ref="C82:H82"/>
-    <mergeCell ref="C83:H83"/>
-    <mergeCell ref="C115:H115"/>
-    <mergeCell ref="C116:H116"/>
-    <mergeCell ref="C121:H121"/>
-    <mergeCell ref="C122:H122"/>
-    <mergeCell ref="C101:H101"/>
-    <mergeCell ref="C107:H107"/>
-    <mergeCell ref="C108:H108"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>